<commit_message>
Applying Multiprocessing to yfinance
</commit_message>
<xml_diff>
--- a/NYSE_profit_헬스케어 업체 및 서비스.xlsx
+++ b/NYSE_profit_헬스케어 업체 및 서비스.xlsx
@@ -14,120 +14,117 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="37">
+  <si>
+    <t>OSH</t>
+  </si>
   <si>
     <t>USPH</t>
   </si>
   <si>
+    <t>AGL</t>
+  </si>
+  <si>
+    <t>SGFY</t>
+  </si>
+  <si>
+    <t>CI</t>
+  </si>
+  <si>
+    <t>CANO</t>
+  </si>
+  <si>
+    <t>SEM</t>
+  </si>
+  <si>
+    <t>HUM</t>
+  </si>
+  <si>
+    <t>UNH</t>
+  </si>
+  <si>
+    <t>AMN</t>
+  </si>
+  <si>
+    <t>ELV</t>
+  </si>
+  <si>
+    <t>CNC</t>
+  </si>
+  <si>
     <t>AMWL</t>
   </si>
   <si>
-    <t>CI</t>
-  </si>
-  <si>
-    <t>OSH</t>
-  </si>
-  <si>
-    <t>SGFY</t>
-  </si>
-  <si>
-    <t>SEM</t>
-  </si>
-  <si>
-    <t>AGL</t>
-  </si>
-  <si>
-    <t>ELV</t>
-  </si>
-  <si>
-    <t>HUM</t>
-  </si>
-  <si>
-    <t>UNH</t>
+    <t>HIMS</t>
+  </si>
+  <si>
+    <t>CHE</t>
   </si>
   <si>
     <t>DGX</t>
   </si>
   <si>
-    <t>AMN</t>
-  </si>
-  <si>
-    <t>CNC</t>
-  </si>
-  <si>
-    <t>CANO</t>
-  </si>
-  <si>
-    <t>CHE</t>
+    <t>MD</t>
+  </si>
+  <si>
+    <t>MOH</t>
+  </si>
+  <si>
+    <t>EHC</t>
   </si>
   <si>
     <t>CVS</t>
   </si>
   <si>
-    <t>HIMS</t>
-  </si>
-  <si>
-    <t>MD</t>
+    <t>LH</t>
   </si>
   <si>
     <t>CCM</t>
   </si>
   <si>
-    <t>MOH</t>
-  </si>
-  <si>
-    <t>LH</t>
+    <t>HNGR</t>
+  </si>
+  <si>
+    <t>DVA</t>
+  </si>
+  <si>
+    <t>FMS</t>
+  </si>
+  <si>
+    <t>ENZ</t>
+  </si>
+  <si>
+    <t>UHS</t>
+  </si>
+  <si>
+    <t>HCA</t>
+  </si>
+  <si>
+    <t>BKD</t>
+  </si>
+  <si>
+    <t>THC</t>
   </si>
   <si>
     <t>ATIP</t>
   </si>
   <si>
-    <t>EHC</t>
-  </si>
-  <si>
-    <t>HNGR</t>
-  </si>
-  <si>
-    <t>FMS</t>
-  </si>
-  <si>
     <t>CO</t>
   </si>
   <si>
-    <t>UHS</t>
-  </si>
-  <si>
-    <t>HCA</t>
-  </si>
-  <si>
-    <t>DVA</t>
-  </si>
-  <si>
-    <t>BKD</t>
-  </si>
-  <si>
-    <t>THC</t>
-  </si>
-  <si>
     <t>SNDA</t>
   </si>
   <si>
-    <t>ENZ</t>
-  </si>
-  <si>
     <t>TDOC</t>
   </si>
   <si>
     <t>CYH</t>
   </si>
   <si>
+    <t>EHAB</t>
+  </si>
+  <si>
     <t>GTS</t>
-  </si>
-  <si>
-    <t>EHC WI</t>
-  </si>
-  <si>
-    <t>EHAB WI</t>
   </si>
 </sst>
 </file>
@@ -485,7 +482,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B39"/>
+  <dimension ref="A1:B38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -501,7 +498,7 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>21.53575570071182</v>
+        <v>36.83608664351632</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -509,7 +506,7 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <v>17.73049637395216</v>
+        <v>32.94926656527903</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -517,7 +514,7 @@
         <v>2</v>
       </c>
       <c r="B4">
-        <v>13.68466531965042</v>
+        <v>30.51434364895804</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -525,7 +522,7 @@
         <v>3</v>
       </c>
       <c r="B5">
-        <v>13.19245822813959</v>
+        <v>17.79358727677658</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -533,7 +530,7 @@
         <v>4</v>
       </c>
       <c r="B6">
-        <v>9.110318260460048</v>
+        <v>16.32858510324024</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -541,7 +538,7 @@
         <v>5</v>
       </c>
       <c r="B7">
-        <v>8.878297638010114</v>
+        <v>16.2217655116502</v>
       </c>
     </row>
     <row r="8" spans="1:2">
@@ -549,7 +546,7 @@
         <v>6</v>
       </c>
       <c r="B8">
-        <v>8.555892721729052</v>
+        <v>15.20588890639578</v>
       </c>
     </row>
     <row r="9" spans="1:2">
@@ -557,7 +554,7 @@
         <v>7</v>
       </c>
       <c r="B9">
-        <v>7.377335377687122</v>
+        <v>12.64756968131993</v>
       </c>
     </row>
     <row r="10" spans="1:2">
@@ -565,7 +562,7 @@
         <v>8</v>
       </c>
       <c r="B10">
-        <v>7.115762929398173</v>
+        <v>12.05001686993969</v>
       </c>
     </row>
     <row r="11" spans="1:2">
@@ -573,7 +570,7 @@
         <v>9</v>
       </c>
       <c r="B11">
-        <v>6.954623767424506</v>
+        <v>10.75937274789458</v>
       </c>
     </row>
     <row r="12" spans="1:2">
@@ -581,7 +578,7 @@
         <v>10</v>
       </c>
       <c r="B12">
-        <v>6.073784309220187</v>
+        <v>8.788034554830194</v>
       </c>
     </row>
     <row r="13" spans="1:2">
@@ -589,7 +586,7 @@
         <v>11</v>
       </c>
       <c r="B13">
-        <v>5.944976064517626</v>
+        <v>8.520940064745508</v>
       </c>
     </row>
     <row r="14" spans="1:2">
@@ -597,7 +594,7 @@
         <v>12</v>
       </c>
       <c r="B14">
-        <v>2.360199568406407</v>
+        <v>7.328603815170709</v>
       </c>
     </row>
     <row r="15" spans="1:2">
@@ -605,7 +602,7 @@
         <v>13</v>
       </c>
       <c r="B15">
-        <v>-0.8213544721353827</v>
+        <v>5.555564182877837</v>
       </c>
     </row>
     <row r="16" spans="1:2">
@@ -613,7 +610,7 @@
         <v>14</v>
       </c>
       <c r="B16">
-        <v>-1.458726116691322</v>
+        <v>5.129939284980667</v>
       </c>
     </row>
     <row r="17" spans="1:2">
@@ -621,7 +618,7 @@
         <v>15</v>
       </c>
       <c r="B17">
-        <v>-8.316335005358644</v>
+        <v>4.511483300821162</v>
       </c>
     </row>
     <row r="18" spans="1:2">
@@ -629,7 +626,7 @@
         <v>16</v>
       </c>
       <c r="B18">
-        <v>-8.812252486564287</v>
+        <v>0.5112946005290997</v>
       </c>
     </row>
     <row r="19" spans="1:2">
@@ -637,7 +634,7 @@
         <v>17</v>
       </c>
       <c r="B19">
-        <v>-9.160629234901252</v>
+        <v>-2.600443378539696</v>
       </c>
     </row>
     <row r="20" spans="1:2">
@@ -645,7 +642,7 @@
         <v>18</v>
       </c>
       <c r="B20">
-        <v>-9.478670067201278</v>
+        <v>-5.212710887194194</v>
       </c>
     </row>
     <row r="21" spans="1:2">
@@ -653,7 +650,7 @@
         <v>19</v>
       </c>
       <c r="B21">
-        <v>-10.52888782634327</v>
+        <v>-7.511410009733233</v>
       </c>
     </row>
     <row r="22" spans="1:2">
@@ -661,7 +658,7 @@
         <v>20</v>
       </c>
       <c r="B22">
-        <v>-10.78178763950419</v>
+        <v>-9.598670445149715</v>
       </c>
     </row>
     <row r="23" spans="1:2">
@@ -669,7 +666,7 @@
         <v>21</v>
       </c>
       <c r="B23">
-        <v>-12.75510179256708</v>
+        <v>-12.32226939244276</v>
       </c>
     </row>
     <row r="24" spans="1:2">
@@ -677,7 +674,7 @@
         <v>22</v>
       </c>
       <c r="B24">
-        <v>-13.85350675025423</v>
+        <v>-18.59823776573276</v>
       </c>
     </row>
     <row r="25" spans="1:2">
@@ -685,7 +682,7 @@
         <v>23</v>
       </c>
       <c r="B25">
-        <v>-17.1081690832906</v>
+        <v>-24.20856276937896</v>
       </c>
     </row>
     <row r="26" spans="1:2">
@@ -693,7 +690,7 @@
         <v>24</v>
       </c>
       <c r="B26">
-        <v>-19.29209275869073</v>
+        <v>-25.60285370411389</v>
       </c>
     </row>
     <row r="27" spans="1:2">
@@ -701,7 +698,7 @@
         <v>25</v>
       </c>
       <c r="B27">
-        <v>-21.92117928642845</v>
+        <v>-27.05166798799355</v>
       </c>
     </row>
     <row r="28" spans="1:2">
@@ -709,7 +706,7 @@
         <v>26</v>
       </c>
       <c r="B28">
-        <v>-24.71100872960008</v>
+        <v>-28.28791380811402</v>
       </c>
     </row>
     <row r="29" spans="1:2">
@@ -717,7 +714,7 @@
         <v>27</v>
       </c>
       <c r="B29">
-        <v>-27.78461209063241</v>
+        <v>-31.08173585568399</v>
       </c>
     </row>
     <row r="30" spans="1:2">
@@ -725,7 +722,7 @@
         <v>28</v>
       </c>
       <c r="B30">
-        <v>-29.55572864576247</v>
+        <v>-34.30232695143178</v>
       </c>
     </row>
     <row r="31" spans="1:2">
@@ -733,7 +730,7 @@
         <v>29</v>
       </c>
       <c r="B31">
-        <v>-29.79651390458517</v>
+        <v>-35.39946433646136</v>
       </c>
     </row>
     <row r="32" spans="1:2">
@@ -741,7 +738,7 @@
         <v>30</v>
       </c>
       <c r="B32">
-        <v>-33.86440243668618</v>
+        <v>-36.22449103716458</v>
       </c>
     </row>
     <row r="33" spans="1:2">
@@ -749,7 +746,7 @@
         <v>31</v>
       </c>
       <c r="B33">
-        <v>-37.23529366885915</v>
+        <v>-37.68472889047156</v>
       </c>
     </row>
     <row r="34" spans="1:2">
@@ -757,7 +754,7 @@
         <v>32</v>
       </c>
       <c r="B34">
-        <v>-38.90577465748163</v>
+        <v>-39.55882577335134</v>
       </c>
     </row>
     <row r="35" spans="1:2">
@@ -765,7 +762,7 @@
         <v>33</v>
       </c>
       <c r="B35">
-        <v>-50.65209158569586</v>
+        <v>-46.5419577481719</v>
       </c>
     </row>
     <row r="36" spans="1:2">
@@ -773,7 +770,7 @@
         <v>34</v>
       </c>
       <c r="B36">
-        <v>-61.08468065159093</v>
+        <v>-65.36631754867777</v>
       </c>
     </row>
     <row r="37" spans="1:2">
@@ -784,11 +781,6 @@
     <row r="38" spans="1:2">
       <c r="A38" s="1" t="s">
         <v>36</v>
-      </c>
-    </row>
-    <row r="39" spans="1:2">
-      <c r="A39" s="1" t="s">
-        <v>37</v>
       </c>
     </row>
   </sheetData>

</xml_diff>